<commit_message>
updates to max number of jobs
</commit_message>
<xml_diff>
--- a/dmsan/bwaise/results/baseline_summary.xlsx
+++ b/dmsan/bwaise/results/baseline_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bfca01abaf64aab7/Coding/ds/dmsan/bwaise/results/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlohm\Dropbox\Lohman-Guest_Shared\12_PhD_Paper3_Sanitation_Decision-Making\Python Code\GitHubDesktop\DMsan\dmsan\bwaise\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="807" documentId="8_{65188E18-495E-0F45-8B78-02B87BA3B559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6EFBCF68-35EF-E240-B632-2C20391B4C3C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C53882-FFB3-43C9-BE0C-66507EFB7025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2380" yWindow="1140" windowWidth="30140" windowHeight="18680" xr2:uid="{30BD56A1-1584-C04C-AAC9-8B0FB171CCD1}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{30BD56A1-1584-C04C-AAC9-8B0FB171CCD1}"/>
   </bookViews>
   <sheets>
     <sheet name="dmsan_calc" sheetId="3" r:id="rId1"/>
@@ -416,7 +416,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -460,12 +460,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
@@ -474,7 +468,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -490,6 +484,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -521,7 +521,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -567,6 +567,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -577,23 +587,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2052,7 +2055,7 @@
                   <c:v>0.35472344387922394</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -2152,7 +2155,7 @@
                   <c:v>0.66715033814579094</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>0.41666666666666669</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0.41666666666666669</c:v>
@@ -2255,7 +2258,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.6</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>0</c:v>
@@ -6917,8 +6920,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1657686" y="6619683"/>
-          <a:ext cx="4564708" cy="7998323"/>
+          <a:off x="1644318" y="6616508"/>
+          <a:ext cx="4511401" cy="8001498"/>
           <a:chOff x="13843001" y="7021951"/>
           <a:chExt cx="4571999" cy="8282705"/>
         </a:xfrm>
@@ -7513,15 +7516,15 @@
   <dimension ref="A1:AL90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C33" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J48" sqref="J48"/>
+      <selection pane="bottomRight" activeCell="W2" sqref="W2:W10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="28"/>
+    <col min="1" max="1" width="10.83203125" style="22"/>
     <col min="6" max="6" width="52" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
@@ -7537,83 +7540,83 @@
     <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A1" s="27" t="s">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.8">
+      <c r="A1" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="B1" s="26" t="s">
+      <c r="B1" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="20" t="s">
         <v>83</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="20" t="s">
         <v>84</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="K1" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="L1" s="20" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="M1" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="N1" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="O1" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="P1" s="26" t="s">
+      <c r="P1" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="Q1" s="26" t="s">
+      <c r="Q1" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="26" t="s">
+      <c r="R1" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="26" t="s">
+      <c r="S1" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="T1" s="26" t="s">
+      <c r="T1" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="U1" s="26" t="s">
+      <c r="U1" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="V1" s="26" t="s">
+      <c r="V1" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="W1" s="26" t="s">
+      <c r="W1" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="X1" s="26" t="s">
+      <c r="X1" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="Y1" s="26" t="s">
+      <c r="Y1" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="Z1" s="26" t="s">
+      <c r="Z1" s="20" t="s">
         <v>91</v>
       </c>
       <c r="AB1" s="5"/>
@@ -7625,8 +7628,8 @@
       <c r="AF1" s="5"/>
       <c r="AG1" s="5"/>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.8">
+      <c r="A2" s="23" t="s">
         <v>94</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -7702,16 +7705,16 @@
       <c r="V2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W2" s="22" t="s">
+      <c r="W2" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="X2" s="19">
+      <c r="X2" s="23">
         <v>0.52503284468438904</v>
       </c>
-      <c r="Y2" s="19">
+      <c r="Y2" s="23">
         <v>0.222768547753664</v>
       </c>
-      <c r="Z2" s="19">
+      <c r="Z2" s="23">
         <v>0.77723145224633505</v>
       </c>
       <c r="AC2" s="2">
@@ -7727,8 +7730,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.8">
+      <c r="A3" s="23"/>
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -7802,10 +7805,10 @@
       <c r="V3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W3" s="22"/>
-      <c r="X3" s="19"/>
-      <c r="Y3" s="19"/>
-      <c r="Z3" s="19"/>
+      <c r="W3" s="27"/>
+      <c r="X3" s="23"/>
+      <c r="Y3" s="23"/>
+      <c r="Z3" s="23"/>
       <c r="AB3" s="2" t="s">
         <v>0</v>
       </c>
@@ -7822,8 +7825,8 @@
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A4" s="19"/>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.8">
+      <c r="A4" s="23"/>
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
@@ -7897,10 +7900,10 @@
       <c r="V4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W4" s="22"/>
-      <c r="X4" s="19"/>
-      <c r="Y4" s="19"/>
-      <c r="Z4" s="19"/>
+      <c r="W4" s="27"/>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="23"/>
+      <c r="Z4" s="23"/>
       <c r="AB4" s="2" t="s">
         <v>1</v>
       </c>
@@ -7917,8 +7920,8 @@
         <v>0.86399999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A5" s="19"/>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.8">
+      <c r="A5" s="23"/>
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
@@ -7992,10 +7995,10 @@
       <c r="V5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W5" s="22"/>
-      <c r="X5" s="19"/>
-      <c r="Y5" s="19"/>
-      <c r="Z5" s="19"/>
+      <c r="W5" s="27"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
       <c r="AB5" s="16" t="s">
         <v>2</v>
       </c>
@@ -8015,8 +8018,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A6" s="19"/>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.8">
+      <c r="A6" s="23"/>
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
@@ -8090,10 +8093,10 @@
       <c r="V6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W6" s="22"/>
-      <c r="X6" s="19"/>
-      <c r="Y6" s="19"/>
-      <c r="Z6" s="19"/>
+      <c r="W6" s="27"/>
+      <c r="X6" s="23"/>
+      <c r="Y6" s="23"/>
+      <c r="Z6" s="23"/>
       <c r="AB6" s="2" t="s">
         <v>3</v>
       </c>
@@ -8110,8 +8113,8 @@
         <v>0.86799999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A7" s="19"/>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.8">
+      <c r="A7" s="23"/>
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
@@ -8185,10 +8188,10 @@
       <c r="V7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="22"/>
-      <c r="X7" s="19"/>
-      <c r="Y7" s="19"/>
-      <c r="Z7" s="19"/>
+      <c r="W7" s="27"/>
+      <c r="X7" s="23"/>
+      <c r="Y7" s="23"/>
+      <c r="Z7" s="23"/>
       <c r="AB7" s="2" t="s">
         <v>4</v>
       </c>
@@ -8205,8 +8208,8 @@
         <v>0.86599999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A8" s="19"/>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.8">
+      <c r="A8" s="23"/>
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
@@ -8280,10 +8283,10 @@
       <c r="V8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W8" s="22"/>
-      <c r="X8" s="19"/>
-      <c r="Y8" s="19"/>
-      <c r="Z8" s="19"/>
+      <c r="W8" s="27"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="23"/>
       <c r="AB8" s="2" t="s">
         <v>5</v>
       </c>
@@ -8300,8 +8303,8 @@
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A9" s="19"/>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.8">
+      <c r="A9" s="23"/>
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
@@ -8375,10 +8378,10 @@
       <c r="V9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W9" s="22"/>
-      <c r="X9" s="19"/>
-      <c r="Y9" s="19"/>
-      <c r="Z9" s="19"/>
+      <c r="W9" s="27"/>
+      <c r="X9" s="23"/>
+      <c r="Y9" s="23"/>
+      <c r="Z9" s="23"/>
       <c r="AB9" s="16" t="s">
         <v>6</v>
       </c>
@@ -8398,8 +8401,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A10" s="19"/>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.8">
+      <c r="A10" s="23"/>
       <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
@@ -8473,10 +8476,10 @@
       <c r="V10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W10" s="22"/>
-      <c r="X10" s="19"/>
-      <c r="Y10" s="19"/>
-      <c r="Z10" s="19"/>
+      <c r="W10" s="27"/>
+      <c r="X10" s="23"/>
+      <c r="Y10" s="23"/>
+      <c r="Z10" s="23"/>
       <c r="AB10" s="2" t="s">
         <v>7</v>
       </c>
@@ -8493,8 +8496,8 @@
         <v>0.872</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.8">
+      <c r="A11" s="24" t="s">
         <v>95</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -8570,16 +8573,16 @@
       <c r="V11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W11" s="23">
+      <c r="W11" s="28">
         <v>10772692659397</v>
       </c>
-      <c r="X11" s="20">
+      <c r="X11" s="24">
         <v>9.2316746113130996E-2</v>
       </c>
-      <c r="Y11" s="20">
+      <c r="Y11" s="24">
         <v>0.64705702498652895</v>
       </c>
-      <c r="Z11" s="20">
+      <c r="Z11" s="24">
         <v>0.47424873507917698</v>
       </c>
       <c r="AB11" s="2" t="s">
@@ -8598,8 +8601,8 @@
         <v>0.873</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.8">
+      <c r="A12" s="24"/>
       <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
@@ -8673,10 +8676,10 @@
       <c r="V12" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="W12" s="23"/>
-      <c r="X12" s="20"/>
-      <c r="Y12" s="20"/>
-      <c r="Z12" s="20"/>
+      <c r="W12" s="28"/>
+      <c r="X12" s="24"/>
+      <c r="Y12" s="24"/>
+      <c r="Z12" s="24"/>
       <c r="AB12" s="2" t="s">
         <v>9</v>
       </c>
@@ -8696,8 +8699,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.8">
+      <c r="A13" s="24"/>
       <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
@@ -8771,10 +8774,10 @@
       <c r="V13" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="W13" s="23"/>
-      <c r="X13" s="20"/>
-      <c r="Y13" s="20"/>
-      <c r="Z13" s="20"/>
+      <c r="W13" s="28"/>
+      <c r="X13" s="24"/>
+      <c r="Y13" s="24"/>
+      <c r="Z13" s="24"/>
       <c r="AB13" s="2" t="s">
         <v>10</v>
       </c>
@@ -8791,8 +8794,8 @@
         <v>0.879</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.8">
+      <c r="A14" s="24"/>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
@@ -8866,10 +8869,10 @@
       <c r="V14" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="W14" s="23"/>
-      <c r="X14" s="20"/>
-      <c r="Y14" s="20"/>
-      <c r="Z14" s="20"/>
+      <c r="W14" s="28"/>
+      <c r="X14" s="24"/>
+      <c r="Y14" s="24"/>
+      <c r="Z14" s="24"/>
       <c r="AB14" s="2" t="s">
         <v>11</v>
       </c>
@@ -8886,8 +8889,8 @@
         <v>0.877</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A15" s="20"/>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.8">
+      <c r="A15" s="24"/>
       <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
@@ -8961,10 +8964,10 @@
       <c r="V15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="W15" s="23"/>
-      <c r="X15" s="20"/>
-      <c r="Y15" s="20"/>
-      <c r="Z15" s="20"/>
+      <c r="W15" s="28"/>
+      <c r="X15" s="24"/>
+      <c r="Y15" s="24"/>
+      <c r="Z15" s="24"/>
       <c r="AB15" s="2" t="s">
         <v>12</v>
       </c>
@@ -8981,8 +8984,8 @@
         <v>0.86699999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.8">
+      <c r="A16" s="24"/>
       <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
@@ -9056,10 +9059,10 @@
       <c r="V16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W16" s="23"/>
-      <c r="X16" s="20"/>
-      <c r="Y16" s="20"/>
-      <c r="Z16" s="20"/>
+      <c r="W16" s="28"/>
+      <c r="X16" s="24"/>
+      <c r="Y16" s="24"/>
+      <c r="Z16" s="24"/>
       <c r="AB16" s="2" t="s">
         <v>13</v>
       </c>
@@ -9079,8 +9082,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.8">
+      <c r="A17" s="25" t="s">
         <v>96</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -9158,16 +9161,16 @@
       <c r="V17" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="W17" s="24">
+      <c r="W17" s="26">
         <v>0</v>
       </c>
-      <c r="X17" s="21">
+      <c r="X17" s="25">
         <v>0.37659429400210898</v>
       </c>
-      <c r="Y17" s="21">
+      <c r="Y17" s="25">
         <v>0.82320173909174899</v>
       </c>
-      <c r="Z17" s="21">
+      <c r="Z17" s="25">
         <v>0.34525479959489402</v>
       </c>
       <c r="AB17" s="2" t="s">
@@ -9186,8 +9189,8 @@
         <v>0.873</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A18" s="21"/>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.8">
+      <c r="A18" s="25"/>
       <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
@@ -9263,10 +9266,10 @@
       <c r="V18" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="W18" s="24"/>
-      <c r="X18" s="21"/>
-      <c r="Y18" s="21"/>
-      <c r="Z18" s="21"/>
+      <c r="W18" s="26"/>
+      <c r="X18" s="25"/>
+      <c r="Y18" s="25"/>
+      <c r="Z18" s="25"/>
       <c r="AB18" s="16" t="s">
         <v>16</v>
       </c>
@@ -9286,8 +9289,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A19" s="21"/>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.8">
+      <c r="A19" s="25"/>
       <c r="B19" s="5" t="s">
         <v>18</v>
       </c>
@@ -9363,10 +9366,10 @@
       <c r="V19" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="W19" s="24"/>
-      <c r="X19" s="21"/>
-      <c r="Y19" s="21"/>
-      <c r="Z19" s="21"/>
+      <c r="W19" s="26"/>
+      <c r="X19" s="25"/>
+      <c r="Y19" s="25"/>
+      <c r="Z19" s="25"/>
       <c r="AB19" s="2" t="s">
         <v>17</v>
       </c>
@@ -9383,8 +9386,8 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A20" s="28" t="s">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.8">
+      <c r="A20" s="22" t="s">
         <v>97</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -9486,8 +9489,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A21" s="21" t="s">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.8">
+      <c r="A21" s="25" t="s">
         <v>98</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -9525,20 +9528,20 @@
       <c r="L21" s="5">
         <v>0</v>
       </c>
-      <c r="M21" s="5">
-        <v>20</v>
+      <c r="M21" s="29">
+        <v>24</v>
       </c>
       <c r="N21" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="O21" s="5">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="P21" s="5">
         <f t="shared" si="0"/>
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="Q21" s="11">
         <f t="shared" si="3"/>
@@ -9563,16 +9566,16 @@
       <c r="V21" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="W21" s="24">
+      <c r="W21" s="26">
         <v>1857053897038.98</v>
       </c>
-      <c r="X21" s="21">
+      <c r="X21" s="25">
         <v>0.38349218128747298</v>
       </c>
-      <c r="Y21" s="21">
+      <c r="Y21" s="25">
         <v>0.98071059257219495</v>
       </c>
-      <c r="Z21" s="21">
+      <c r="Z21" s="25">
         <v>1.9289407427804401E-2</v>
       </c>
       <c r="AB21" s="3" t="s">
@@ -9585,8 +9588,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A22" s="21"/>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.8">
+      <c r="A22" s="25"/>
       <c r="B22" s="5" t="s">
         <v>20</v>
       </c>
@@ -9622,7 +9625,7 @@
       <c r="L22" s="5">
         <v>0</v>
       </c>
-      <c r="M22" s="5">
+      <c r="M22" s="29">
         <v>12</v>
       </c>
       <c r="N22" s="5">
@@ -9660,10 +9663,10 @@
       <c r="V22" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="W22" s="24"/>
-      <c r="X22" s="21"/>
-      <c r="Y22" s="21"/>
-      <c r="Z22" s="21"/>
+      <c r="W22" s="26"/>
+      <c r="X22" s="25"/>
+      <c r="Y22" s="25"/>
+      <c r="Z22" s="25"/>
       <c r="AB22" s="2" t="s">
         <v>19</v>
       </c>
@@ -9680,8 +9683,8 @@
         <v>0.86699999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A23" s="21"/>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.8">
+      <c r="A23" s="25"/>
       <c r="B23" s="7" t="s">
         <v>21</v>
       </c>
@@ -9755,10 +9758,10 @@
       <c r="V23" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="W23" s="24"/>
-      <c r="X23" s="21"/>
-      <c r="Y23" s="21"/>
-      <c r="Z23" s="21"/>
+      <c r="W23" s="26"/>
+      <c r="X23" s="25"/>
+      <c r="Y23" s="25"/>
+      <c r="Z23" s="25"/>
       <c r="AB23" s="3" t="s">
         <v>20</v>
       </c>
@@ -9775,8 +9778,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A24" s="21"/>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.8">
+      <c r="A24" s="25"/>
       <c r="B24" s="5" t="s">
         <v>22</v>
       </c>
@@ -9850,10 +9853,10 @@
       <c r="V24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="W24" s="24"/>
-      <c r="X24" s="21"/>
-      <c r="Y24" s="21"/>
-      <c r="Z24" s="21"/>
+      <c r="W24" s="26"/>
+      <c r="X24" s="25"/>
+      <c r="Y24" s="25"/>
+      <c r="Z24" s="25"/>
       <c r="AB24" s="16" t="s">
         <v>21</v>
       </c>
@@ -9873,8 +9876,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A25" s="21"/>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.8">
+      <c r="A25" s="25"/>
       <c r="B25" s="5" t="s">
         <v>23</v>
       </c>
@@ -9948,10 +9951,10 @@
       <c r="V25" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="W25" s="24"/>
-      <c r="X25" s="21"/>
-      <c r="Y25" s="21"/>
-      <c r="Z25" s="21"/>
+      <c r="W25" s="26"/>
+      <c r="X25" s="25"/>
+      <c r="Y25" s="25"/>
+      <c r="Z25" s="25"/>
       <c r="AB25" s="2" t="s">
         <v>22</v>
       </c>
@@ -9968,8 +9971,8 @@
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.8">
+      <c r="A26" s="25"/>
       <c r="B26" s="5" t="s">
         <v>24</v>
       </c>
@@ -10043,10 +10046,10 @@
       <c r="V26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="W26" s="24"/>
-      <c r="X26" s="21"/>
-      <c r="Y26" s="21"/>
-      <c r="Z26" s="21"/>
+      <c r="W26" s="26"/>
+      <c r="X26" s="25"/>
+      <c r="Y26" s="25"/>
+      <c r="Z26" s="25"/>
       <c r="AB26" s="2" t="s">
         <v>23</v>
       </c>
@@ -10063,8 +10066,8 @@
         <v>0.88100000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A27" s="21"/>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.8">
+      <c r="A27" s="25"/>
       <c r="B27" s="5" t="s">
         <v>25</v>
       </c>
@@ -10138,10 +10141,10 @@
       <c r="V27" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="W27" s="24"/>
-      <c r="X27" s="21"/>
-      <c r="Y27" s="21"/>
-      <c r="Z27" s="21"/>
+      <c r="W27" s="26"/>
+      <c r="X27" s="25"/>
+      <c r="Y27" s="25"/>
+      <c r="Z27" s="25"/>
       <c r="AB27" s="2" t="s">
         <v>24</v>
       </c>
@@ -10158,8 +10161,8 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A28" s="21"/>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.8">
+      <c r="A28" s="25"/>
       <c r="B28" s="7" t="s">
         <v>26</v>
       </c>
@@ -10203,10 +10206,10 @@
       <c r="T28" s="7"/>
       <c r="U28" s="7"/>
       <c r="V28" s="5"/>
-      <c r="W28" s="24"/>
-      <c r="X28" s="21"/>
-      <c r="Y28" s="21"/>
-      <c r="Z28" s="21"/>
+      <c r="W28" s="26"/>
+      <c r="X28" s="25"/>
+      <c r="Y28" s="25"/>
+      <c r="Z28" s="25"/>
       <c r="AB28" s="2" t="s">
         <v>25</v>
       </c>
@@ -10223,8 +10226,8 @@
         <v>0.877</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A29" s="21"/>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.8">
+      <c r="A29" s="25"/>
       <c r="B29" s="7" t="s">
         <v>27</v>
       </c>
@@ -10268,10 +10271,10 @@
       <c r="T29" s="7"/>
       <c r="U29" s="7"/>
       <c r="V29" s="5"/>
-      <c r="W29" s="24"/>
-      <c r="X29" s="21"/>
-      <c r="Y29" s="21"/>
-      <c r="Z29" s="21"/>
+      <c r="W29" s="26"/>
+      <c r="X29" s="25"/>
+      <c r="Y29" s="25"/>
+      <c r="Z29" s="25"/>
       <c r="AB29" s="5"/>
       <c r="AC29" s="5"/>
       <c r="AD29" s="5"/>
@@ -10287,7 +10290,7 @@
       <c r="AJ29" s="5"/>
       <c r="AK29" s="5"/>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.8">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -10320,14 +10323,14 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.8">
       <c r="B31" t="s">
         <v>67</v>
       </c>
       <c r="C31">
         <v>0</v>
       </c>
-      <c r="N31" s="25" t="s">
+      <c r="N31" s="19" t="s">
         <v>92</v>
       </c>
       <c r="O31" s="1"/>
@@ -10348,8 +10351,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="N32" s="25" t="s">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.8">
+      <c r="N32" s="19" t="s">
         <v>93</v>
       </c>
       <c r="O32" s="1"/>
@@ -10370,7 +10373,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="33" spans="14:32" x14ac:dyDescent="0.2">
+    <row r="33" spans="14:32" x14ac:dyDescent="0.8">
       <c r="N33">
         <v>0.66666666666666596</v>
       </c>
@@ -10396,7 +10399,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="34" spans="14:32" x14ac:dyDescent="0.2">
+    <row r="34" spans="14:32" x14ac:dyDescent="0.8">
       <c r="N34">
         <v>0.57735026918962495</v>
       </c>
@@ -10422,7 +10425,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="35" spans="14:32" x14ac:dyDescent="0.2">
+    <row r="35" spans="14:32" x14ac:dyDescent="0.8">
       <c r="N35">
         <v>0.61545745489666304</v>
       </c>
@@ -10448,7 +10451,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="36" spans="14:32" x14ac:dyDescent="0.2">
+    <row r="36" spans="14:32" x14ac:dyDescent="0.8">
       <c r="N36">
         <v>0.53916386601719202</v>
       </c>
@@ -10474,7 +10477,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="37" spans="14:32" x14ac:dyDescent="0.2">
+    <row r="37" spans="14:32" x14ac:dyDescent="0.8">
       <c r="N37">
         <v>0.68041381743977103</v>
       </c>
@@ -10500,7 +10503,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="38" spans="14:32" x14ac:dyDescent="0.2">
+    <row r="38" spans="14:32" x14ac:dyDescent="0.8">
       <c r="N38">
         <v>0.63960214906683099</v>
       </c>
@@ -10526,7 +10529,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="39" spans="14:32" x14ac:dyDescent="0.2">
+    <row r="39" spans="14:32" x14ac:dyDescent="0.8">
       <c r="N39">
         <v>0.57735026918962495</v>
       </c>
@@ -10552,7 +10555,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="40" spans="14:32" x14ac:dyDescent="0.2">
+    <row r="40" spans="14:32" x14ac:dyDescent="0.8">
       <c r="N40">
         <v>0.57735026918962495</v>
       </c>
@@ -10578,7 +10581,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="41" spans="14:32" x14ac:dyDescent="0.2">
+    <row r="41" spans="14:32" x14ac:dyDescent="0.8">
       <c r="N41">
         <v>0.40824829046386302</v>
       </c>
@@ -10604,7 +10607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="14:32" x14ac:dyDescent="0.2">
+    <row r="42" spans="14:32" x14ac:dyDescent="0.8">
       <c r="N42">
         <v>0</v>
       </c>
@@ -10630,7 +10633,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="43" spans="14:32" x14ac:dyDescent="0.2">
+    <row r="43" spans="14:32" x14ac:dyDescent="0.8">
       <c r="N43">
         <v>0.111622790427321</v>
       </c>
@@ -10656,7 +10659,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="44" spans="14:32" x14ac:dyDescent="0.2">
+    <row r="44" spans="14:32" x14ac:dyDescent="0.8">
       <c r="N44">
         <v>0.38840611238939798</v>
       </c>
@@ -10682,7 +10685,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="45" spans="14:32" x14ac:dyDescent="0.2">
+    <row r="45" spans="14:32" x14ac:dyDescent="0.8">
       <c r="N45">
         <v>0.52625762130341802</v>
       </c>
@@ -10708,7 +10711,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="14:32" x14ac:dyDescent="0.2">
+    <row r="46" spans="14:32" x14ac:dyDescent="0.8">
       <c r="N46">
         <v>0</v>
       </c>
@@ -10734,7 +10737,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="47" spans="14:32" x14ac:dyDescent="0.2">
+    <row r="47" spans="14:32" x14ac:dyDescent="0.8">
       <c r="N47">
         <v>0.48507125007266499</v>
       </c>
@@ -10760,7 +10763,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="48" spans="14:32" x14ac:dyDescent="0.2">
+    <row r="48" spans="14:32" x14ac:dyDescent="0.8">
       <c r="N48">
         <v>-0.21869141911503501</v>
       </c>
@@ -10786,7 +10789,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="49" spans="13:38" x14ac:dyDescent="0.2">
+    <row r="49" spans="13:38" x14ac:dyDescent="0.8">
       <c r="N49">
         <v>-0.142819206327576</v>
       </c>
@@ -10806,7 +10809,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="50" spans="13:38" x14ac:dyDescent="0.2">
+    <row r="50" spans="13:38" x14ac:dyDescent="0.8">
       <c r="N50">
         <v>2.84594191251385E-2</v>
       </c>
@@ -10823,7 +10826,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="51" spans="13:38" x14ac:dyDescent="0.2">
+    <row r="51" spans="13:38" x14ac:dyDescent="0.8">
       <c r="N51">
         <v>0.52215818581535001</v>
       </c>
@@ -10849,7 +10852,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="52" spans="13:38" x14ac:dyDescent="0.2">
+    <row r="52" spans="13:38" x14ac:dyDescent="0.8">
       <c r="N52">
         <v>0.60920769908017103</v>
       </c>
@@ -10872,7 +10875,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="53" spans="13:38" x14ac:dyDescent="0.2">
+    <row r="53" spans="13:38" x14ac:dyDescent="0.8">
       <c r="N53">
         <v>0</v>
       </c>
@@ -10898,7 +10901,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="54" spans="13:38" x14ac:dyDescent="0.2">
+    <row r="54" spans="13:38" x14ac:dyDescent="0.8">
       <c r="N54">
         <v>1.1984579651951901E-2</v>
       </c>
@@ -10924,7 +10927,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="55" spans="13:38" x14ac:dyDescent="0.2">
+    <row r="55" spans="13:38" x14ac:dyDescent="0.8">
       <c r="N55">
         <v>0.69631062382279096</v>
       </c>
@@ -10950,7 +10953,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="56" spans="13:38" x14ac:dyDescent="0.2">
+    <row r="56" spans="13:38" x14ac:dyDescent="0.8">
       <c r="N56">
         <v>0.57735026918962495</v>
       </c>
@@ -10976,7 +10979,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="57" spans="13:38" x14ac:dyDescent="0.2">
+    <row r="57" spans="13:38" x14ac:dyDescent="0.8">
       <c r="N57">
         <v>0.61545745489666304</v>
       </c>
@@ -11002,7 +11005,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="58" spans="13:38" x14ac:dyDescent="0.2">
+    <row r="58" spans="13:38" x14ac:dyDescent="0.8">
       <c r="M58" s="13"/>
       <c r="N58">
         <v>0.57735026918962495</v>
@@ -11019,7 +11022,7 @@
       <c r="AK58" s="13"/>
       <c r="AL58" s="13"/>
     </row>
-    <row r="59" spans="13:38" x14ac:dyDescent="0.2">
+    <row r="59" spans="13:38" x14ac:dyDescent="0.8">
       <c r="N59" s="13">
         <v>0</v>
       </c>
@@ -11030,7 +11033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="13:38" x14ac:dyDescent="0.2">
+    <row r="60" spans="13:38" x14ac:dyDescent="0.8">
       <c r="N60">
         <v>0</v>
       </c>
@@ -11041,33 +11044,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="8:10" x14ac:dyDescent="0.2">
+    <row r="84" spans="8:10" x14ac:dyDescent="0.8">
       <c r="H84" s="13"/>
       <c r="J84" s="13"/>
     </row>
-    <row r="86" spans="8:10" x14ac:dyDescent="0.2">
+    <row r="86" spans="8:10" x14ac:dyDescent="0.8">
       <c r="H86" s="13"/>
       <c r="J86" s="13"/>
     </row>
-    <row r="88" spans="8:10" x14ac:dyDescent="0.2">
+    <row r="88" spans="8:10" x14ac:dyDescent="0.8">
       <c r="H88" s="13"/>
       <c r="J88" s="13"/>
     </row>
-    <row r="89" spans="8:10" x14ac:dyDescent="0.2">
+    <row r="89" spans="8:10" x14ac:dyDescent="0.8">
       <c r="H89" s="13"/>
       <c r="J89" s="13"/>
     </row>
-    <row r="90" spans="8:10" x14ac:dyDescent="0.2">
+    <row r="90" spans="8:10" x14ac:dyDescent="0.8">
       <c r="H90" s="13"/>
       <c r="J90" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A11:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A21:A29"/>
-    <mergeCell ref="W17:W19"/>
+    <mergeCell ref="X2:X10"/>
+    <mergeCell ref="Y2:Y10"/>
+    <mergeCell ref="Z2:Z10"/>
+    <mergeCell ref="W11:W16"/>
+    <mergeCell ref="X11:X16"/>
+    <mergeCell ref="Y11:Y16"/>
+    <mergeCell ref="Z11:Z16"/>
     <mergeCell ref="X17:X19"/>
     <mergeCell ref="Y17:Y19"/>
     <mergeCell ref="Z17:Z19"/>
@@ -11075,14 +11080,12 @@
     <mergeCell ref="X21:X29"/>
     <mergeCell ref="Y21:Y29"/>
     <mergeCell ref="Z21:Z29"/>
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A21:A29"/>
+    <mergeCell ref="W17:W19"/>
     <mergeCell ref="W2:W10"/>
-    <mergeCell ref="X2:X10"/>
-    <mergeCell ref="Y2:Y10"/>
-    <mergeCell ref="Z2:Z10"/>
-    <mergeCell ref="W11:W16"/>
-    <mergeCell ref="X11:X16"/>
-    <mergeCell ref="Y11:Y16"/>
-    <mergeCell ref="Z11:Z16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11096,7 +11099,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
checkpoint on consistency check (done with AHP indicator weights)
</commit_message>
<xml_diff>
--- a/dmsan/bwaise/results/baseline_summary.xlsx
+++ b/dmsan/bwaise/results/baseline_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlohm\Dropbox\Lohman-Guest_Shared\12_PhD_Paper3_Sanitation_Decision-Making\Python Code\GitHubDesktop\DMsan\dmsan\bwaise\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yalinli_cabbi/Library/CloudStorage/OneDrive-Personal/Coding/ds/dmsan/bwaise/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7C53882-FFB3-43C9-BE0C-66507EFB7025}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750EE62A-17ED-814F-ADB6-2FD2C2B68244}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{30BD56A1-1584-C04C-AAC9-8B0FB171CCD1}"/>
+    <workbookView xWindow="3540" yWindow="8100" windowWidth="28800" windowHeight="18000" xr2:uid="{30BD56A1-1584-C04C-AAC9-8B0FB171CCD1}"/>
   </bookViews>
   <sheets>
     <sheet name="dmsan_calc" sheetId="3" r:id="rId1"/>
@@ -40,8 +40,6 @@
     <author>tc={B5F27424-D0D3-E94D-9F5E-1734972EA681}</author>
     <author>tc={19CAAF9C-03C8-6845-8613-F6E1D651E63E}</author>
     <author>tc={E6336642-3446-AF49-A2BF-3B09F9EAC343}</author>
-    <author>tc={6643E3E3-32E6-0048-BAB6-23CD6C7EC166}</author>
-    <author>tc={5B6C309A-26C9-5344-90EB-EA8D801E71F1}</author>
     <author>tc={7E65E023-2B6F-5747-934C-C0E8EBBE617E}</author>
   </authors>
   <commentList>
@@ -69,23 +67,7 @@
     Note that we only considered energy in biogas (not COD in liquids/solids, so the results are different from the comparison_summary.xlsx in EXPOsan, but it is consistent with John’s results in exposan/bwaise/comparison/uncertainty/Bwaise_sanitation_outputs_uncertaintyB.xlsx</t>
       </text>
     </comment>
-    <comment ref="I16" authorId="3" shapeId="0" xr:uid="{6643E3E3-32E6-0048-BAB6-23CD6C7EC166}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    inconsistent with the SI</t>
-      </text>
-    </comment>
-    <comment ref="L16" authorId="4" shapeId="0" xr:uid="{5B6C309A-26C9-5344-90EB-EA8D801E71F1}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    4 in the SI</t>
-      </text>
-    </comment>
-    <comment ref="M20" authorId="5" shapeId="0" xr:uid="{7E65E023-2B6F-5747-934C-C0E8EBBE617E}">
+    <comment ref="M20" authorId="3" shapeId="0" xr:uid="{7E65E023-2B6F-5747-934C-C0E8EBBE617E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -577,7 +559,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -591,12 +579,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -847,7 +829,7 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -955,7 +937,7 @@
                   <c:v>0.25</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1064,7 +1046,7 @@
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -1457,7 +1439,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
@@ -1672,7 +1654,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5</c:v>
+                  <c:v>0.33333333333333331</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>1</c:v>
@@ -6920,8 +6902,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="1644318" y="6616508"/>
-          <a:ext cx="4511401" cy="8001498"/>
+          <a:off x="1644318" y="6619683"/>
+          <a:ext cx="4524602" cy="7998323"/>
           <a:chOff x="13843001" y="7021951"/>
           <a:chExt cx="4571999" cy="8282705"/>
         </a:xfrm>
@@ -7499,12 +7481,6 @@
   <threadedComment ref="F15" dT="2021-12-19T17:09:05.20" personId="{146A595A-F3AA-FD4D-BA51-55B8CEA152BB}" id="{E6336642-3446-AF49-A2BF-3B09F9EAC343}">
     <text>Note that we only considered energy in biogas (not COD in liquids/solids, so the results are different from the comparison_summary.xlsx in EXPOsan, but it is consistent with John’s results in exposan/bwaise/comparison/uncertainty/Bwaise_sanitation_outputs_uncertaintyB.xlsx</text>
   </threadedComment>
-  <threadedComment ref="I16" dT="2021-12-18T22:12:16.62" personId="{146A595A-F3AA-FD4D-BA51-55B8CEA152BB}" id="{6643E3E3-32E6-0048-BAB6-23CD6C7EC166}">
-    <text>inconsistent with the SI</text>
-  </threadedComment>
-  <threadedComment ref="L16" dT="2021-12-18T22:11:59.47" personId="{146A595A-F3AA-FD4D-BA51-55B8CEA152BB}" id="{5B6C309A-26C9-5344-90EB-EA8D801E71F1}">
-    <text>4 in the SI</text>
-  </threadedComment>
   <threadedComment ref="M20" dT="2021-12-18T22:14:00.22" personId="{146A595A-F3AA-FD4D-BA51-55B8CEA152BB}" id="{7E65E023-2B6F-5747-934C-C0E8EBBE617E}">
     <text>why is this 0 rather than the minimum? not consistent with the other simulated indicators, and why can’t cost be negative?</text>
   </threadedComment>
@@ -7516,13 +7492,13 @@
   <dimension ref="A1:AL90"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="W2" sqref="W2:W10"/>
+      <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="22"/>
     <col min="6" max="6" width="52" bestFit="1" customWidth="1"/>
@@ -7540,7 +7516,7 @@
     <col min="26" max="26" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.2">
       <c r="A1" s="21" t="s">
         <v>99</v>
       </c>
@@ -7628,8 +7604,8 @@
       <c r="AF1" s="5"/>
       <c r="AG1" s="5"/>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.8">
-      <c r="A2" s="23" t="s">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A2" s="24" t="s">
         <v>94</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -7705,16 +7681,16 @@
       <c r="V2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W2" s="27" t="s">
+      <c r="W2" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="X2" s="23">
+      <c r="X2" s="24">
         <v>0.52503284468438904</v>
       </c>
-      <c r="Y2" s="23">
+      <c r="Y2" s="24">
         <v>0.222768547753664</v>
       </c>
-      <c r="Z2" s="23">
+      <c r="Z2" s="24">
         <v>0.77723145224633505</v>
       </c>
       <c r="AC2" s="2">
@@ -7730,8 +7706,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.8">
-      <c r="A3" s="23"/>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A3" s="24"/>
       <c r="B3" s="5" t="s">
         <v>1</v>
       </c>
@@ -7805,10 +7781,10 @@
       <c r="V3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W3" s="27"/>
-      <c r="X3" s="23"/>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="23"/>
+      <c r="W3" s="29"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
       <c r="AB3" s="2" t="s">
         <v>0</v>
       </c>
@@ -7825,8 +7801,8 @@
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.8">
-      <c r="A4" s="23"/>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A4" s="24"/>
       <c r="B4" s="5" t="s">
         <v>2</v>
       </c>
@@ -7900,10 +7876,10 @@
       <c r="V4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W4" s="27"/>
-      <c r="X4" s="23"/>
-      <c r="Y4" s="23"/>
-      <c r="Z4" s="23"/>
+      <c r="W4" s="29"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
       <c r="AB4" s="2" t="s">
         <v>1</v>
       </c>
@@ -7920,8 +7896,8 @@
         <v>0.86399999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.8">
-      <c r="A5" s="23"/>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A5" s="24"/>
       <c r="B5" s="5" t="s">
         <v>3</v>
       </c>
@@ -7995,10 +7971,10 @@
       <c r="V5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W5" s="27"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
+      <c r="W5" s="29"/>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="24"/>
+      <c r="Z5" s="24"/>
       <c r="AB5" s="16" t="s">
         <v>2</v>
       </c>
@@ -8018,8 +7994,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.8">
-      <c r="A6" s="23"/>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A6" s="24"/>
       <c r="B6" s="5" t="s">
         <v>4</v>
       </c>
@@ -8093,10 +8069,10 @@
       <c r="V6" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W6" s="27"/>
-      <c r="X6" s="23"/>
-      <c r="Y6" s="23"/>
-      <c r="Z6" s="23"/>
+      <c r="W6" s="29"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="24"/>
       <c r="AB6" s="2" t="s">
         <v>3</v>
       </c>
@@ -8113,8 +8089,8 @@
         <v>0.86799999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.8">
-      <c r="A7" s="23"/>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A7" s="24"/>
       <c r="B7" s="5" t="s">
         <v>5</v>
       </c>
@@ -8188,10 +8164,10 @@
       <c r="V7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W7" s="27"/>
-      <c r="X7" s="23"/>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="23"/>
+      <c r="W7" s="29"/>
+      <c r="X7" s="24"/>
+      <c r="Y7" s="24"/>
+      <c r="Z7" s="24"/>
       <c r="AB7" s="2" t="s">
         <v>4</v>
       </c>
@@ -8208,8 +8184,8 @@
         <v>0.86599999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.8">
-      <c r="A8" s="23"/>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A8" s="24"/>
       <c r="B8" s="5" t="s">
         <v>6</v>
       </c>
@@ -8246,19 +8222,19 @@
         <v>1</v>
       </c>
       <c r="M8" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N8" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="O8" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P8" s="5">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="Q8" s="11">
         <f t="shared" si="3"/>
@@ -8283,10 +8259,10 @@
       <c r="V8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W8" s="27"/>
-      <c r="X8" s="23"/>
-      <c r="Y8" s="23"/>
-      <c r="Z8" s="23"/>
+      <c r="W8" s="29"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="24"/>
+      <c r="Z8" s="24"/>
       <c r="AB8" s="2" t="s">
         <v>5</v>
       </c>
@@ -8303,8 +8279,8 @@
         <v>0.86899999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.8">
-      <c r="A9" s="23"/>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A9" s="24"/>
       <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
@@ -8378,10 +8354,10 @@
       <c r="V9" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W9" s="27"/>
-      <c r="X9" s="23"/>
-      <c r="Y9" s="23"/>
-      <c r="Z9" s="23"/>
+      <c r="W9" s="29"/>
+      <c r="X9" s="24"/>
+      <c r="Y9" s="24"/>
+      <c r="Z9" s="24"/>
       <c r="AB9" s="16" t="s">
         <v>6</v>
       </c>
@@ -8401,8 +8377,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.8">
-      <c r="A10" s="23"/>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A10" s="24"/>
       <c r="B10" s="5" t="s">
         <v>8</v>
       </c>
@@ -8476,10 +8452,10 @@
       <c r="V10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W10" s="27"/>
-      <c r="X10" s="23"/>
-      <c r="Y10" s="23"/>
-      <c r="Z10" s="23"/>
+      <c r="W10" s="29"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="24"/>
+      <c r="Z10" s="24"/>
       <c r="AB10" s="2" t="s">
         <v>7</v>
       </c>
@@ -8496,8 +8472,8 @@
         <v>0.872</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.8">
-      <c r="A11" s="24" t="s">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A11" s="26" t="s">
         <v>95</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -8573,16 +8549,16 @@
       <c r="V11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W11" s="28">
+      <c r="W11" s="25">
         <v>10772692659397</v>
       </c>
-      <c r="X11" s="24">
+      <c r="X11" s="26">
         <v>9.2316746113130996E-2</v>
       </c>
-      <c r="Y11" s="24">
+      <c r="Y11" s="26">
         <v>0.64705702498652895</v>
       </c>
-      <c r="Z11" s="24">
+      <c r="Z11" s="26">
         <v>0.47424873507917698</v>
       </c>
       <c r="AB11" s="2" t="s">
@@ -8601,8 +8577,8 @@
         <v>0.873</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.8">
-      <c r="A12" s="24"/>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A12" s="26"/>
       <c r="B12" s="5" t="s">
         <v>10</v>
       </c>
@@ -8676,10 +8652,10 @@
       <c r="V12" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="W12" s="28"/>
-      <c r="X12" s="24"/>
-      <c r="Y12" s="24"/>
-      <c r="Z12" s="24"/>
+      <c r="W12" s="25"/>
+      <c r="X12" s="26"/>
+      <c r="Y12" s="26"/>
+      <c r="Z12" s="26"/>
       <c r="AB12" s="2" t="s">
         <v>9</v>
       </c>
@@ -8699,8 +8675,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.8">
-      <c r="A13" s="24"/>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A13" s="26"/>
       <c r="B13" s="5" t="s">
         <v>11</v>
       </c>
@@ -8774,10 +8750,10 @@
       <c r="V13" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="W13" s="28"/>
-      <c r="X13" s="24"/>
-      <c r="Y13" s="24"/>
-      <c r="Z13" s="24"/>
+      <c r="W13" s="25"/>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="26"/>
+      <c r="Z13" s="26"/>
       <c r="AB13" s="2" t="s">
         <v>10</v>
       </c>
@@ -8794,8 +8770,8 @@
         <v>0.879</v>
       </c>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.8">
-      <c r="A14" s="24"/>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A14" s="26"/>
       <c r="B14" s="5" t="s">
         <v>12</v>
       </c>
@@ -8869,10 +8845,10 @@
       <c r="V14" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="W14" s="28"/>
-      <c r="X14" s="24"/>
-      <c r="Y14" s="24"/>
-      <c r="Z14" s="24"/>
+      <c r="W14" s="25"/>
+      <c r="X14" s="26"/>
+      <c r="Y14" s="26"/>
+      <c r="Z14" s="26"/>
       <c r="AB14" s="2" t="s">
         <v>11</v>
       </c>
@@ -8889,8 +8865,8 @@
         <v>0.877</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.8">
-      <c r="A15" s="24"/>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A15" s="26"/>
       <c r="B15" s="5" t="s">
         <v>13</v>
       </c>
@@ -8964,10 +8940,10 @@
       <c r="V15" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="W15" s="28"/>
-      <c r="X15" s="24"/>
-      <c r="Y15" s="24"/>
-      <c r="Z15" s="24"/>
+      <c r="W15" s="25"/>
+      <c r="X15" s="26"/>
+      <c r="Y15" s="26"/>
+      <c r="Z15" s="26"/>
       <c r="AB15" s="2" t="s">
         <v>12</v>
       </c>
@@ -8984,8 +8960,8 @@
         <v>0.86699999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.8">
-      <c r="A16" s="24"/>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.2">
+      <c r="A16" s="26"/>
       <c r="B16" s="5" t="s">
         <v>14</v>
       </c>
@@ -9010,23 +8986,23 @@
         <v>0.119567342176383</v>
       </c>
       <c r="I16" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J16" s="6">
+        <v>4</v>
+      </c>
+      <c r="K16" s="6">
         <v>3</v>
       </c>
-      <c r="K16" s="6">
-        <v>2</v>
-      </c>
       <c r="L16" s="6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M16" s="5">
         <v>1</v>
       </c>
       <c r="N16" s="5">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="O16" s="5">
         <f t="shared" si="0"/>
@@ -9034,15 +9010,15 @@
       </c>
       <c r="P16" s="5">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="Q16" s="11">
         <f>MAX(I16:K16)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R16" s="11">
         <f>MIN(I16:K16)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S16" s="11">
         <f t="shared" si="5"/>
@@ -9059,10 +9035,10 @@
       <c r="V16" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="W16" s="28"/>
-      <c r="X16" s="24"/>
-      <c r="Y16" s="24"/>
-      <c r="Z16" s="24"/>
+      <c r="W16" s="25"/>
+      <c r="X16" s="26"/>
+      <c r="Y16" s="26"/>
+      <c r="Z16" s="26"/>
       <c r="AB16" s="2" t="s">
         <v>13</v>
       </c>
@@ -9082,8 +9058,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="17" spans="1:37" x14ac:dyDescent="0.8">
-      <c r="A17" s="25" t="s">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A17" s="27" t="s">
         <v>96</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -9161,16 +9137,16 @@
       <c r="V17" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="W17" s="26">
+      <c r="W17" s="28">
         <v>0</v>
       </c>
-      <c r="X17" s="25">
+      <c r="X17" s="27">
         <v>0.37659429400210898</v>
       </c>
-      <c r="Y17" s="25">
+      <c r="Y17" s="27">
         <v>0.82320173909174899</v>
       </c>
-      <c r="Z17" s="25">
+      <c r="Z17" s="27">
         <v>0.34525479959489402</v>
       </c>
       <c r="AB17" s="2" t="s">
@@ -9189,8 +9165,8 @@
         <v>0.873</v>
       </c>
     </row>
-    <row r="18" spans="1:37" x14ac:dyDescent="0.8">
-      <c r="A18" s="25"/>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A18" s="27"/>
       <c r="B18" s="5" t="s">
         <v>17</v>
       </c>
@@ -9266,10 +9242,10 @@
       <c r="V18" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="W18" s="26"/>
-      <c r="X18" s="25"/>
-      <c r="Y18" s="25"/>
-      <c r="Z18" s="25"/>
+      <c r="W18" s="28"/>
+      <c r="X18" s="27"/>
+      <c r="Y18" s="27"/>
+      <c r="Z18" s="27"/>
       <c r="AB18" s="16" t="s">
         <v>16</v>
       </c>
@@ -9289,8 +9265,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="19" spans="1:37" x14ac:dyDescent="0.8">
-      <c r="A19" s="25"/>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A19" s="27"/>
       <c r="B19" s="5" t="s">
         <v>18</v>
       </c>
@@ -9366,10 +9342,10 @@
       <c r="V19" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="W19" s="26"/>
-      <c r="X19" s="25"/>
-      <c r="Y19" s="25"/>
-      <c r="Z19" s="25"/>
+      <c r="W19" s="28"/>
+      <c r="X19" s="27"/>
+      <c r="Y19" s="27"/>
+      <c r="Z19" s="27"/>
       <c r="AB19" s="2" t="s">
         <v>17</v>
       </c>
@@ -9386,7 +9362,7 @@
         <v>0.875</v>
       </c>
     </row>
-    <row r="20" spans="1:37" x14ac:dyDescent="0.8">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A20" s="22" t="s">
         <v>97</v>
       </c>
@@ -9489,8 +9465,8 @@
         <v>69</v>
       </c>
     </row>
-    <row r="21" spans="1:37" x14ac:dyDescent="0.8">
-      <c r="A21" s="25" t="s">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A21" s="27" t="s">
         <v>98</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -9528,7 +9504,7 @@
       <c r="L21" s="5">
         <v>0</v>
       </c>
-      <c r="M21" s="29">
+      <c r="M21" s="23">
         <v>24</v>
       </c>
       <c r="N21" s="5">
@@ -9566,16 +9542,16 @@
       <c r="V21" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="W21" s="26">
+      <c r="W21" s="28">
         <v>1857053897038.98</v>
       </c>
-      <c r="X21" s="25">
+      <c r="X21" s="27">
         <v>0.38349218128747298</v>
       </c>
-      <c r="Y21" s="25">
+      <c r="Y21" s="27">
         <v>0.98071059257219495</v>
       </c>
-      <c r="Z21" s="25">
+      <c r="Z21" s="27">
         <v>1.9289407427804401E-2</v>
       </c>
       <c r="AB21" s="3" t="s">
@@ -9588,8 +9564,8 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:37" x14ac:dyDescent="0.8">
-      <c r="A22" s="25"/>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A22" s="27"/>
       <c r="B22" s="5" t="s">
         <v>20</v>
       </c>
@@ -9625,7 +9601,7 @@
       <c r="L22" s="5">
         <v>0</v>
       </c>
-      <c r="M22" s="29">
+      <c r="M22" s="23">
         <v>12</v>
       </c>
       <c r="N22" s="5">
@@ -9663,10 +9639,10 @@
       <c r="V22" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="W22" s="26"/>
-      <c r="X22" s="25"/>
-      <c r="Y22" s="25"/>
-      <c r="Z22" s="25"/>
+      <c r="W22" s="28"/>
+      <c r="X22" s="27"/>
+      <c r="Y22" s="27"/>
+      <c r="Z22" s="27"/>
       <c r="AB22" s="2" t="s">
         <v>19</v>
       </c>
@@ -9683,8 +9659,8 @@
         <v>0.86699999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:37" x14ac:dyDescent="0.8">
-      <c r="A23" s="25"/>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A23" s="27"/>
       <c r="B23" s="7" t="s">
         <v>21</v>
       </c>
@@ -9758,10 +9734,10 @@
       <c r="V23" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="W23" s="26"/>
-      <c r="X23" s="25"/>
-      <c r="Y23" s="25"/>
-      <c r="Z23" s="25"/>
+      <c r="W23" s="28"/>
+      <c r="X23" s="27"/>
+      <c r="Y23" s="27"/>
+      <c r="Z23" s="27"/>
       <c r="AB23" s="3" t="s">
         <v>20</v>
       </c>
@@ -9778,8 +9754,8 @@
         <v>70</v>
       </c>
     </row>
-    <row r="24" spans="1:37" x14ac:dyDescent="0.8">
-      <c r="A24" s="25"/>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A24" s="27"/>
       <c r="B24" s="5" t="s">
         <v>22</v>
       </c>
@@ -9853,10 +9829,10 @@
       <c r="V24" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="W24" s="26"/>
-      <c r="X24" s="25"/>
-      <c r="Y24" s="25"/>
-      <c r="Z24" s="25"/>
+      <c r="W24" s="28"/>
+      <c r="X24" s="27"/>
+      <c r="Y24" s="27"/>
+      <c r="Z24" s="27"/>
       <c r="AB24" s="16" t="s">
         <v>21</v>
       </c>
@@ -9876,8 +9852,8 @@
         <v>78</v>
       </c>
     </row>
-    <row r="25" spans="1:37" x14ac:dyDescent="0.8">
-      <c r="A25" s="25"/>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A25" s="27"/>
       <c r="B25" s="5" t="s">
         <v>23</v>
       </c>
@@ -9951,10 +9927,10 @@
       <c r="V25" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="W25" s="26"/>
-      <c r="X25" s="25"/>
-      <c r="Y25" s="25"/>
-      <c r="Z25" s="25"/>
+      <c r="W25" s="28"/>
+      <c r="X25" s="27"/>
+      <c r="Y25" s="27"/>
+      <c r="Z25" s="27"/>
       <c r="AB25" s="2" t="s">
         <v>22</v>
       </c>
@@ -9971,8 +9947,8 @@
         <v>0.88800000000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:37" x14ac:dyDescent="0.8">
-      <c r="A26" s="25"/>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A26" s="27"/>
       <c r="B26" s="5" t="s">
         <v>24</v>
       </c>
@@ -10046,10 +10022,10 @@
       <c r="V26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="W26" s="26"/>
-      <c r="X26" s="25"/>
-      <c r="Y26" s="25"/>
-      <c r="Z26" s="25"/>
+      <c r="W26" s="28"/>
+      <c r="X26" s="27"/>
+      <c r="Y26" s="27"/>
+      <c r="Z26" s="27"/>
       <c r="AB26" s="2" t="s">
         <v>23</v>
       </c>
@@ -10066,8 +10042,8 @@
         <v>0.88100000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:37" x14ac:dyDescent="0.8">
-      <c r="A27" s="25"/>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A27" s="27"/>
       <c r="B27" s="5" t="s">
         <v>25</v>
       </c>
@@ -10141,10 +10117,10 @@
       <c r="V27" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="W27" s="26"/>
-      <c r="X27" s="25"/>
-      <c r="Y27" s="25"/>
-      <c r="Z27" s="25"/>
+      <c r="W27" s="28"/>
+      <c r="X27" s="27"/>
+      <c r="Y27" s="27"/>
+      <c r="Z27" s="27"/>
       <c r="AB27" s="2" t="s">
         <v>24</v>
       </c>
@@ -10161,8 +10137,8 @@
         <v>0.87</v>
       </c>
     </row>
-    <row r="28" spans="1:37" x14ac:dyDescent="0.8">
-      <c r="A28" s="25"/>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A28" s="27"/>
       <c r="B28" s="7" t="s">
         <v>26</v>
       </c>
@@ -10206,10 +10182,10 @@
       <c r="T28" s="7"/>
       <c r="U28" s="7"/>
       <c r="V28" s="5"/>
-      <c r="W28" s="26"/>
-      <c r="X28" s="25"/>
-      <c r="Y28" s="25"/>
-      <c r="Z28" s="25"/>
+      <c r="W28" s="28"/>
+      <c r="X28" s="27"/>
+      <c r="Y28" s="27"/>
+      <c r="Z28" s="27"/>
       <c r="AB28" s="2" t="s">
         <v>25</v>
       </c>
@@ -10226,8 +10202,8 @@
         <v>0.877</v>
       </c>
     </row>
-    <row r="29" spans="1:37" x14ac:dyDescent="0.8">
-      <c r="A29" s="25"/>
+    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="A29" s="27"/>
       <c r="B29" s="7" t="s">
         <v>27</v>
       </c>
@@ -10271,10 +10247,10 @@
       <c r="T29" s="7"/>
       <c r="U29" s="7"/>
       <c r="V29" s="5"/>
-      <c r="W29" s="26"/>
-      <c r="X29" s="25"/>
-      <c r="Y29" s="25"/>
-      <c r="Z29" s="25"/>
+      <c r="W29" s="28"/>
+      <c r="X29" s="27"/>
+      <c r="Y29" s="27"/>
+      <c r="Z29" s="27"/>
       <c r="AB29" s="5"/>
       <c r="AC29" s="5"/>
       <c r="AD29" s="5"/>
@@ -10290,7 +10266,7 @@
       <c r="AJ29" s="5"/>
       <c r="AK29" s="5"/>
     </row>
-    <row r="30" spans="1:37" x14ac:dyDescent="0.8">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5"/>
@@ -10323,7 +10299,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:37" x14ac:dyDescent="0.8">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>67</v>
       </c>
@@ -10351,7 +10327,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:37" x14ac:dyDescent="0.8">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
       <c r="N32" s="19" t="s">
         <v>93</v>
       </c>
@@ -10373,7 +10349,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="33" spans="14:32" x14ac:dyDescent="0.8">
+    <row r="33" spans="14:32" x14ac:dyDescent="0.2">
       <c r="N33">
         <v>0.66666666666666596</v>
       </c>
@@ -10399,7 +10375,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="34" spans="14:32" x14ac:dyDescent="0.8">
+    <row r="34" spans="14:32" x14ac:dyDescent="0.2">
       <c r="N34">
         <v>0.57735026918962495</v>
       </c>
@@ -10425,7 +10401,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="35" spans="14:32" x14ac:dyDescent="0.8">
+    <row r="35" spans="14:32" x14ac:dyDescent="0.2">
       <c r="N35">
         <v>0.61545745489666304</v>
       </c>
@@ -10451,7 +10427,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="36" spans="14:32" x14ac:dyDescent="0.8">
+    <row r="36" spans="14:32" x14ac:dyDescent="0.2">
       <c r="N36">
         <v>0.53916386601719202</v>
       </c>
@@ -10477,7 +10453,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="37" spans="14:32" x14ac:dyDescent="0.8">
+    <row r="37" spans="14:32" x14ac:dyDescent="0.2">
       <c r="N37">
         <v>0.68041381743977103</v>
       </c>
@@ -10503,7 +10479,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="38" spans="14:32" x14ac:dyDescent="0.8">
+    <row r="38" spans="14:32" x14ac:dyDescent="0.2">
       <c r="N38">
         <v>0.63960214906683099</v>
       </c>
@@ -10529,7 +10505,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="39" spans="14:32" x14ac:dyDescent="0.8">
+    <row r="39" spans="14:32" x14ac:dyDescent="0.2">
       <c r="N39">
         <v>0.57735026918962495</v>
       </c>
@@ -10555,7 +10531,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="40" spans="14:32" x14ac:dyDescent="0.8">
+    <row r="40" spans="14:32" x14ac:dyDescent="0.2">
       <c r="N40">
         <v>0.57735026918962495</v>
       </c>
@@ -10581,7 +10557,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="41" spans="14:32" x14ac:dyDescent="0.8">
+    <row r="41" spans="14:32" x14ac:dyDescent="0.2">
       <c r="N41">
         <v>0.40824829046386302</v>
       </c>
@@ -10607,7 +10583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="14:32" x14ac:dyDescent="0.8">
+    <row r="42" spans="14:32" x14ac:dyDescent="0.2">
       <c r="N42">
         <v>0</v>
       </c>
@@ -10633,7 +10609,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="43" spans="14:32" x14ac:dyDescent="0.8">
+    <row r="43" spans="14:32" x14ac:dyDescent="0.2">
       <c r="N43">
         <v>0.111622790427321</v>
       </c>
@@ -10659,7 +10635,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="44" spans="14:32" x14ac:dyDescent="0.8">
+    <row r="44" spans="14:32" x14ac:dyDescent="0.2">
       <c r="N44">
         <v>0.38840611238939798</v>
       </c>
@@ -10685,7 +10661,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="45" spans="14:32" x14ac:dyDescent="0.8">
+    <row r="45" spans="14:32" x14ac:dyDescent="0.2">
       <c r="N45">
         <v>0.52625762130341802</v>
       </c>
@@ -10711,7 +10687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="14:32" x14ac:dyDescent="0.8">
+    <row r="46" spans="14:32" x14ac:dyDescent="0.2">
       <c r="N46">
         <v>0</v>
       </c>
@@ -10737,7 +10713,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="47" spans="14:32" x14ac:dyDescent="0.8">
+    <row r="47" spans="14:32" x14ac:dyDescent="0.2">
       <c r="N47">
         <v>0.48507125007266499</v>
       </c>
@@ -10763,7 +10739,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="48" spans="14:32" x14ac:dyDescent="0.8">
+    <row r="48" spans="14:32" x14ac:dyDescent="0.2">
       <c r="N48">
         <v>-0.21869141911503501</v>
       </c>
@@ -10789,7 +10765,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="49" spans="13:38" x14ac:dyDescent="0.8">
+    <row r="49" spans="13:38" x14ac:dyDescent="0.2">
       <c r="N49">
         <v>-0.142819206327576</v>
       </c>
@@ -10809,7 +10785,7 @@
         <v>0.61</v>
       </c>
     </row>
-    <row r="50" spans="13:38" x14ac:dyDescent="0.8">
+    <row r="50" spans="13:38" x14ac:dyDescent="0.2">
       <c r="N50">
         <v>2.84594191251385E-2</v>
       </c>
@@ -10826,7 +10802,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="51" spans="13:38" x14ac:dyDescent="0.8">
+    <row r="51" spans="13:38" x14ac:dyDescent="0.2">
       <c r="N51">
         <v>0.52215818581535001</v>
       </c>
@@ -10852,7 +10828,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="52" spans="13:38" x14ac:dyDescent="0.8">
+    <row r="52" spans="13:38" x14ac:dyDescent="0.2">
       <c r="N52">
         <v>0.60920769908017103</v>
       </c>
@@ -10875,7 +10851,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="53" spans="13:38" x14ac:dyDescent="0.8">
+    <row r="53" spans="13:38" x14ac:dyDescent="0.2">
       <c r="N53">
         <v>0</v>
       </c>
@@ -10901,7 +10877,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="54" spans="13:38" x14ac:dyDescent="0.8">
+    <row r="54" spans="13:38" x14ac:dyDescent="0.2">
       <c r="N54">
         <v>1.1984579651951901E-2</v>
       </c>
@@ -10927,7 +10903,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="55" spans="13:38" x14ac:dyDescent="0.8">
+    <row r="55" spans="13:38" x14ac:dyDescent="0.2">
       <c r="N55">
         <v>0.69631062382279096</v>
       </c>
@@ -10953,7 +10929,7 @@
         <v>0.89</v>
       </c>
     </row>
-    <row r="56" spans="13:38" x14ac:dyDescent="0.8">
+    <row r="56" spans="13:38" x14ac:dyDescent="0.2">
       <c r="N56">
         <v>0.57735026918962495</v>
       </c>
@@ -10979,7 +10955,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="57" spans="13:38" x14ac:dyDescent="0.8">
+    <row r="57" spans="13:38" x14ac:dyDescent="0.2">
       <c r="N57">
         <v>0.61545745489666304</v>
       </c>
@@ -11005,7 +10981,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="58" spans="13:38" x14ac:dyDescent="0.8">
+    <row r="58" spans="13:38" x14ac:dyDescent="0.2">
       <c r="M58" s="13"/>
       <c r="N58">
         <v>0.57735026918962495</v>
@@ -11022,7 +10998,7 @@
       <c r="AK58" s="13"/>
       <c r="AL58" s="13"/>
     </row>
-    <row r="59" spans="13:38" x14ac:dyDescent="0.8">
+    <row r="59" spans="13:38" x14ac:dyDescent="0.2">
       <c r="N59" s="13">
         <v>0</v>
       </c>
@@ -11033,7 +11009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="13:38" x14ac:dyDescent="0.8">
+    <row r="60" spans="13:38" x14ac:dyDescent="0.2">
       <c r="N60">
         <v>0</v>
       </c>
@@ -11044,28 +11020,41 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="8:10" x14ac:dyDescent="0.8">
+    <row r="84" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H84" s="13"/>
       <c r="J84" s="13"/>
     </row>
-    <row r="86" spans="8:10" x14ac:dyDescent="0.8">
+    <row r="86" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H86" s="13"/>
       <c r="J86" s="13"/>
     </row>
-    <row r="88" spans="8:10" x14ac:dyDescent="0.8">
+    <row r="88" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H88" s="13"/>
       <c r="J88" s="13"/>
     </row>
-    <row r="89" spans="8:10" x14ac:dyDescent="0.8">
+    <row r="89" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H89" s="13"/>
       <c r="J89" s="13"/>
     </row>
-    <row r="90" spans="8:10" x14ac:dyDescent="0.8">
+    <row r="90" spans="8:10" x14ac:dyDescent="0.2">
       <c r="H90" s="13"/>
       <c r="J90" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A2:A10"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A21:A29"/>
+    <mergeCell ref="W17:W19"/>
+    <mergeCell ref="W2:W10"/>
+    <mergeCell ref="X17:X19"/>
+    <mergeCell ref="Y17:Y19"/>
+    <mergeCell ref="Z17:Z19"/>
+    <mergeCell ref="W21:W29"/>
+    <mergeCell ref="X21:X29"/>
+    <mergeCell ref="Y21:Y29"/>
+    <mergeCell ref="Z21:Z29"/>
     <mergeCell ref="X2:X10"/>
     <mergeCell ref="Y2:Y10"/>
     <mergeCell ref="Z2:Z10"/>
@@ -11073,19 +11062,6 @@
     <mergeCell ref="X11:X16"/>
     <mergeCell ref="Y11:Y16"/>
     <mergeCell ref="Z11:Z16"/>
-    <mergeCell ref="X17:X19"/>
-    <mergeCell ref="Y17:Y19"/>
-    <mergeCell ref="Z17:Z19"/>
-    <mergeCell ref="W21:W29"/>
-    <mergeCell ref="X21:X29"/>
-    <mergeCell ref="Y21:Y29"/>
-    <mergeCell ref="Z21:Z29"/>
-    <mergeCell ref="A2:A10"/>
-    <mergeCell ref="A11:A16"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="A21:A29"/>
-    <mergeCell ref="W17:W19"/>
-    <mergeCell ref="W2:W10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -11099,7 +11075,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>